<commit_message>
Atualização de projeto, implementação dos testes cadastro, consulta de produto tela principal, consulta de produto por pesquisa
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/appium/tdd/testdata/TestData.xlsx
+++ b/src/main/java/br/com/rsinet/appium/tdd/testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilker.nogueira\eclipse-workspace-automacao\avaliacao-automacao-tdd-appium\src\main\java\br\com\rsinet\appium\tdd\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1332B7-2732-46A2-9AE2-5AA492D80307}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDAB8AA7-DF2C-4F9A-8169-3BC93F840B0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{8A0BD1D9-DBE4-467F-9B03-07923CE60D62}"/>
   </bookViews>
@@ -283,7 +283,7 @@
     <t>REGISTER</t>
   </si>
   <si>
-    <t>Wilker000031</t>
+    <t>Wilker000032</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Atualizacao, alterado scroll para forma genérica e removido sleep
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/appium/tdd/testdata/TestData.xlsx
+++ b/src/main/java/br/com/rsinet/appium/tdd/testdata/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilker.nogueira\eclipse-workspace-automacao\avaliacao-automacao-tdd-appium\src\main\java\br\com\rsinet\appium\tdd\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDAB8AA7-DF2C-4F9A-8169-3BC93F840B0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB0701E-4697-427F-9E7F-89C82E1330AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{8A0BD1D9-DBE4-467F-9B03-07923CE60D62}"/>
+    <workbookView xWindow="4905" yWindow="1350" windowWidth="15375" windowHeight="7875" firstSheet="1" activeTab="1" xr2:uid="{8A0BD1D9-DBE4-467F-9B03-07923CE60D62}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -283,7 +283,7 @@
     <t>REGISTER</t>
   </si>
   <si>
-    <t>Wilker000032</t>
+    <t>Wilker000036</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Atualizacao de Page para Screen
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/appium/tdd/testdata/TestData.xlsx
+++ b/src/main/java/br/com/rsinet/appium/tdd/testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilker.nogueira\eclipse-workspace-automacao\avaliacao-automacao-tdd-appium\src\main\java\br\com\rsinet\appium\tdd\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB0701E-4697-427F-9E7F-89C82E1330AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70C97F4-3D56-4E13-B280-AEC6C138EEFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4905" yWindow="1350" windowWidth="15375" windowHeight="7875" firstSheet="1" activeTab="1" xr2:uid="{8A0BD1D9-DBE4-467F-9B03-07923CE60D62}"/>
   </bookViews>
@@ -283,7 +283,7 @@
     <t>REGISTER</t>
   </si>
   <si>
-    <t>Wilker000036</t>
+    <t>Wilker000074</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Atualizacao de drivers, todos centralizados no Factory.
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/appium/tdd/testdata/TestData.xlsx
+++ b/src/main/java/br/com/rsinet/appium/tdd/testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilker.nogueira\eclipse-workspace-automacao\avaliacao-automacao-tdd-appium\src\main\java\br\com\rsinet\appium\tdd\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA805F56-F116-4431-A13A-18E16A0BF127}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EBA7FE3-E045-482C-82CC-33F24858F5BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4905" yWindow="1350" windowWidth="15375" windowHeight="7875" firstSheet="1" activeTab="1" xr2:uid="{8A0BD1D9-DBE4-467F-9B03-07923CE60D62}"/>
   </bookViews>
@@ -283,7 +283,7 @@
     <t>REGISTER</t>
   </si>
   <si>
-    <t>Wilker000078</t>
+    <t>Wil0002</t>
   </si>
 </sst>
 </file>

</xml_diff>